<commit_message>
subiendo archivos en github
</commit_message>
<xml_diff>
--- a/Automatizacion/Archivo/Archivo.xlsx
+++ b/Automatizacion/Archivo/Archivo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diana\eclipse-workspace\Automatizacion\Archivo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diana\eclipse-workspace\Automatizacion1\Archivo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -34,7 +34,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Email;deisy.Saenz3@gmail.com;FirtName;Deisy;LastName;Tipazoca;Password;132547;Fname;Deisy;Lname;Tipazoca;Addres;Cra 26 #65-43;City;Colombia;Mobile;1456855;State;Alaska;ZipCode;44454;Country;United States;</t>
+    <t>Email;deisy.Saenz5@gmail.com;FirtName;Deisy;LastName;Tipazoca;Password;132547;Fname;Deisy;Lname;Tipazoca;Addres;Cra 26 #65-43;City;Colombia;Mobile;1456855;State;Alaska;ZipCode;44454;Country;United States;</t>
   </si>
 </sst>
 </file>
@@ -426,7 +426,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>